<commit_message>
Supplier and manufacturer completed
</commit_message>
<xml_diff>
--- a/Utils/Deepam_Dataset.xlsx
+++ b/Utils/Deepam_Dataset.xlsx
@@ -4,10 +4,13 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="17500" windowHeight="6420"/>
+    <workbookView windowWidth="17500" windowHeight="6420" firstSheet="2" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
+    <sheet name="PharmacyAdmin_Supplier" sheetId="2" r:id="rId2"/>
+    <sheet name="PharmacyAdmin_Manufacturer" sheetId="3" r:id="rId3"/>
+    <sheet name="PharmacyAdmin_ProductCategory" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -27,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="40">
   <si>
     <t>URL</t>
   </si>
@@ -63,6 +66,90 @@
   </si>
   <si>
     <t>PharmacyAdmin</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>EmailId</t>
+  </si>
+  <si>
+    <t>Address1</t>
+  </si>
+  <si>
+    <t>Address2</t>
+  </si>
+  <si>
+    <t>City</t>
+  </si>
+  <si>
+    <t>Toast</t>
+  </si>
+  <si>
+    <t>Search</t>
+  </si>
+  <si>
+    <t>arun</t>
+  </si>
+  <si>
+    <t>arun@gmail.com</t>
+  </si>
+  <si>
+    <t>chitlapakkam</t>
+  </si>
+  <si>
+    <t>Chennai</t>
+  </si>
+  <si>
+    <t>Tambaram</t>
+  </si>
+  <si>
+    <t>Supplier created successfully</t>
+  </si>
+  <si>
+    <t>Arun</t>
+  </si>
+  <si>
+    <t>arungmail.com</t>
+  </si>
+  <si>
+    <t>Supplier details updated successfully</t>
+  </si>
+  <si>
+    <t>arunkumar</t>
+  </si>
+  <si>
+    <t>Supplier details deleted successfully</t>
+  </si>
+  <si>
+    <t>RAKPSD</t>
+  </si>
+  <si>
+    <t>Manufacture created successfully</t>
+  </si>
+  <si>
+    <t>YaanMed</t>
+  </si>
+  <si>
+    <t>Manufacture updated successfully</t>
+  </si>
+  <si>
+    <t>Datayaan</t>
+  </si>
+  <si>
+    <t>Manufacturer deleted successfully</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Homeopathyies</t>
+  </si>
+  <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>Homeopathy</t>
   </si>
 </sst>
 </file>
@@ -75,7 +162,7 @@
     <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="23">
+  <fonts count="24">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -84,9 +171,25 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -107,14 +210,6 @@
       <sz val="10.5"/>
       <name val="Consolas"/>
       <charset val="134"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -565,150 +660,159 @@
     <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="6">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="6" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="6">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="6" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="6" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1246,7 +1350,7 @@
   <sheetPr/>
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
@@ -1271,46 +1375,46 @@
       </c>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C2">
         <v>8870822001</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="3"/>
+      <c r="E2" s="6"/>
     </row>
     <row r="3" spans="2:5">
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="3"/>
+      <c r="E3" s="6"/>
     </row>
     <row r="4" spans="2:4">
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="3"/>
+      <c r="D4" s="6"/>
     </row>
     <row r="5" spans="2:4">
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="3"/>
+      <c r="D5" s="6"/>
     </row>
     <row r="6" spans="2:4">
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="3"/>
+      <c r="D6" s="6"/>
     </row>
     <row r="7" spans="2:4">
       <c r="B7" t="s">
@@ -1319,22 +1423,22 @@
       <c r="C7">
         <v>7094755145</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D7" s="5" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="8" spans="2:4">
-      <c r="B8" s="2"/>
-      <c r="D8" s="3"/>
+      <c r="B8" s="5"/>
+      <c r="D8" s="6"/>
     </row>
     <row r="9" spans="2:2">
-      <c r="B9" s="2"/>
+      <c r="B9" s="5"/>
     </row>
     <row r="10" spans="2:2">
-      <c r="B10" s="2"/>
+      <c r="B10" s="5"/>
     </row>
     <row r="11" spans="2:2">
-      <c r="B11" s="2"/>
+      <c r="B11" s="5"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1346,4 +1450,334 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:H4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K4" sqref="K4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5" outlineLevelRow="3" outlineLevelCol="7"/>
+  <cols>
+    <col min="2" max="2" width="11.7272727272727"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="A1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" ht="58" spans="1:8">
+      <c r="A2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2">
+        <v>7082767623</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" ht="72.5" spans="1:7">
+      <c r="A3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3">
+        <v>3082767623</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F3" t="s">
+        <v>23</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" ht="72.5" spans="1:7">
+      <c r="A4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4">
+        <v>7094755143</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" t="s">
+        <v>22</v>
+      </c>
+      <c r="F4" t="s">
+        <v>23</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" display="arun@gmail.com"/>
+    <hyperlink ref="C3" r:id="rId1" display="arungmail.com"/>
+    <hyperlink ref="C4" r:id="rId1" display="arun@gmail.com"/>
+  </hyperlinks>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:H4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O2" sqref="O2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5" outlineLevelRow="3" outlineLevelCol="7"/>
+  <cols>
+    <col min="2" max="2" width="11.7272727272727"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="A1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" ht="72.5" spans="1:8">
+      <c r="A2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2">
+        <v>7082767623</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="H2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" ht="72.5" spans="1:7">
+      <c r="A3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B3">
+        <v>3082767623</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F3" t="s">
+        <v>23</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" ht="72.5" spans="1:8">
+      <c r="A4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B4">
+        <v>7094755143</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" t="s">
+        <v>22</v>
+      </c>
+      <c r="F4" t="s">
+        <v>23</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="H4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" display="arun@gmail.com"/>
+    <hyperlink ref="C3" r:id="rId1" display="arungmail.com"/>
+    <hyperlink ref="C4" r:id="rId1" display="arun@gmail.com"/>
+  </hyperlinks>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:H4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M3" sqref="M3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5" outlineLevelRow="3" outlineLevelCol="7"/>
+  <cols>
+    <col min="2" max="2" width="11.7272727272727"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="A1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+    </row>
+    <row r="2" ht="72.5" spans="1:7">
+      <c r="A2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D2"/>
+      <c r="E2"/>
+      <c r="F2"/>
+      <c r="G2" s="2"/>
+    </row>
+    <row r="3" ht="72.5" spans="1:7">
+      <c r="A3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D3"/>
+      <c r="E3"/>
+      <c r="F3"/>
+      <c r="G3" s="2"/>
+    </row>
+    <row r="4" ht="72.5" spans="1:7">
+      <c r="A4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D4"/>
+      <c r="E4"/>
+      <c r="F4"/>
+      <c r="G4" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
 </file>
</xml_diff>